<commit_message>
Moved use case scenarios into their own files separated by use case.
Also updated the the log.txt file. Pulled in the completed Sprint 3 backlog. Removed old and outdated files.
</commit_message>
<xml_diff>
--- a/sprints/sprint3/Sprint 3 Backlog.xlsx
+++ b/sprints/sprint3/Sprint 3 Backlog.xlsx
@@ -146,7 +146,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -183,11 +183,19 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="8.0"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,12 +234,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF1C232"/>
-        <bgColor rgb="FFF1C232"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF6AA84F"/>
         <bgColor rgb="FF6AA84F"/>
       </patternFill>
@@ -255,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -289,13 +291,13 @@
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -304,21 +306,24 @@
     <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -334,38 +339,41 @@
     <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -695,9 +703,15 @@
       <c r="E5" s="14">
         <v>3.0</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="F5" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0.0</v>
+      </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -716,7 +730,7 @@
       <c r="C6" s="12">
         <v>10.0</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="14">
@@ -725,8 +739,12 @@
       <c r="F6" s="14">
         <v>10.0</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.0</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -745,7 +763,7 @@
       <c r="C7" s="12">
         <v>12.0</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="14">
@@ -754,8 +772,12 @@
       <c r="F7" s="14">
         <v>12.0</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="G7" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0.0</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -767,8 +789,8 @@
       <c r="Q7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="18"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="7">
@@ -780,9 +802,15 @@
       <c r="E8" s="20">
         <v>1.0</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="F8" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="H8" s="21">
+        <v>0.0</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -794,14 +822,14 @@
       <c r="Q8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="18"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="10"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -814,8 +842,8 @@
     </row>
     <row r="10">
       <c r="A10" s="15"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -835,23 +863,27 @@
       <c r="A11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="7">
         <v>9.0</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="21">
         <v>9.0</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="21">
         <v>9.0</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0.0</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -863,12 +895,12 @@
       <c r="Q11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="12"/>
-      <c r="D12" s="24"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -884,12 +916,12 @@
       <c r="Q12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="18"/>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="24"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -905,12 +937,12 @@
       <c r="Q13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="18"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="18" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="24"/>
+      <c r="D14" s="25"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -926,12 +958,12 @@
       <c r="Q14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="18"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="7"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="25"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -947,10 +979,10 @@
       <c r="Q15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="18"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="10"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="24"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -966,16 +998,16 @@
       <c r="Q16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="7">
         <v>5.0</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="25" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="14">
@@ -984,8 +1016,12 @@
       <c r="F17" s="14">
         <v>0.0</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="G17" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H17" s="14">
+        <v>0.0</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -997,14 +1033,14 @@
       <c r="Q17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="18"/>
-      <c r="B18" s="26" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="7">
         <v>2.0</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="25" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="14">
@@ -1013,8 +1049,12 @@
       <c r="F18" s="14">
         <v>0.0</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="G18" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H18" s="14">
+        <v>0.0</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -1027,15 +1067,15 @@
     </row>
     <row r="19">
       <c r="A19" s="9"/>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -1048,23 +1088,27 @@
     </row>
     <row r="20">
       <c r="A20" s="9"/>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="27" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="7">
         <v>3.0</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="29">
+      <c r="E20" s="21">
         <v>3.0</v>
       </c>
-      <c r="F20" s="29">
-        <v>0.0</v>
-      </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="F20" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="G20" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="H20" s="21">
+        <v>0.0</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1080,35 +1124,31 @@
       <c r="B21" s="10"/>
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
-      <c r="O21" s="28">
-        <v>1.0</v>
-      </c>
-      <c r="P21" s="28">
-        <v>69.0</v>
-      </c>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
       <c r="Q21" s="4"/>
     </row>
     <row r="22">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="7">
         <v>11.0</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>33</v>
       </c>
       <c r="E22" s="20">
@@ -1117,8 +1157,12 @@
       <c r="F22" s="20">
         <v>0.0</v>
       </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="G22" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="H22" s="21">
+        <v>0.0</v>
+      </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1130,14 +1174,14 @@
       <c r="Q22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="18"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="7">
         <v>3.0</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="20">
@@ -1146,8 +1190,12 @@
       <c r="F23" s="20">
         <v>0.0</v>
       </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="G23" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="H23" s="21">
+        <v>0.0</v>
+      </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -1159,14 +1207,14 @@
       <c r="Q23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="18"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="30" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="7">
         <v>7.0</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="20">
@@ -1175,8 +1223,12 @@
       <c r="F24" s="20">
         <v>0.0</v>
       </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="G24" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="H24" s="21">
+        <v>0.0</v>
+      </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -1188,14 +1240,14 @@
       <c r="Q24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="31"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -1210,21 +1262,27 @@
       <c r="A26" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="18" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="7">
         <v>3.0</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E26" s="20">
         <v>3.0</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="F26" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="G26" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="H26" s="21">
+        <v>0.0</v>
+      </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -1236,22 +1294,28 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27">
-      <c r="A27" s="18"/>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="18" t="s">
         <v>38</v>
       </c>
       <c r="C27" s="7">
         <v>2.0</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="20">
         <v>2.0</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="F27" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="G27" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="H27" s="21">
+        <v>0.0</v>
+      </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -1263,14 +1327,14 @@
       <c r="Q27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="18"/>
-      <c r="B28" s="22"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="31"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -1282,14 +1346,14 @@
       <c r="Q28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="18"/>
-      <c r="B29" s="22"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="31"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -1301,14 +1365,14 @@
       <c r="Q29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="18"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="31"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -1320,14 +1384,14 @@
       <c r="Q30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="18"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="31"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -1339,24 +1403,30 @@
       <c r="Q31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="18" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="7">
         <v>2.0</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E32" s="20">
         <v>2.0</v>
       </c>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
+      <c r="F32" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="G32" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="H32" s="21">
+        <v>0.0</v>
+      </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -1369,21 +1439,27 @@
     </row>
     <row r="33">
       <c r="A33" s="34"/>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C33" s="7">
         <v>2.0</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="19" t="s">
         <v>13</v>
       </c>
       <c r="E33" s="20">
         <v>2.0</v>
       </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
+      <c r="F33" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="G33" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="H33" s="21">
+        <v>0.0</v>
+      </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -1395,26 +1471,22 @@
       <c r="Q33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="31"/>
       <c r="D34" s="8"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
-      <c r="O34" s="28">
-        <v>4.0</v>
-      </c>
-      <c r="P34" s="28">
-        <v>0.0</v>
-      </c>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
       <c r="Q34" s="4"/>
     </row>
     <row r="35">
@@ -1426,10 +1498,20 @@
         <v>77</v>
       </c>
       <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
+      <c r="E35" s="36">
+        <f t="shared" ref="E35:F35" si="1">SUM(E5:E33)</f>
+        <v>54</v>
+      </c>
+      <c r="F35" s="36">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="G35" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H35" s="36">
+        <v>0.0</v>
+      </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -1537,8 +1619,12 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
+      <c r="H41" s="37">
+        <v>4.0</v>
+      </c>
+      <c r="I41" s="37">
+        <v>77.0</v>
+      </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
@@ -1555,8 +1641,12 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
+      <c r="H42" s="37">
+        <v>3.0</v>
+      </c>
+      <c r="I42" s="37">
+        <v>54.0</v>
+      </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
@@ -1574,8 +1664,12 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
+      <c r="H43" s="37">
+        <v>2.0</v>
+      </c>
+      <c r="I43" s="37">
+        <v>40.0</v>
+      </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
@@ -1587,6 +1681,12 @@
     </row>
     <row r="44">
       <c r="A44" s="4"/>
+      <c r="H44" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="I44" s="38">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="4"/>

</xml_diff>